<commit_message>
Generate a configurable number or doubles
</commit_message>
<xml_diff>
--- a/ServicesLayer/FirstRun/Data/Config.xlsx
+++ b/ServicesLayer/FirstRun/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>If &gt; 0 will retry the Initialisation state with a failed exception.</t>
+  </si>
+  <si>
+    <t>FillNumber</t>
+  </si>
+  <si>
+    <t>How many doubles to genrate</t>
   </si>
 </sst>
 </file>
@@ -585,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -676,7 +682,17 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1678,7 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE325D7-4482-47A6-A6F6-6E2DBC946231}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Framework Level exceptions are now full output (exception.ToString).
</commit_message>
<xml_diff>
--- a/ServicesLayer/FirstRun/Data/Config.xlsx
+++ b/ServicesLayer/FirstRun/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>58</v>
       </c>
       <c r="B7" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE325D7-4482-47A6-A6F6-6E2DBC946231}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bug where businessRuleException would go to init
</commit_message>
<xml_diff>
--- a/ServicesLayer/FirstRun/Data/Config.xlsx
+++ b/ServicesLayer/FirstRun/Data/Config.xlsx
@@ -594,7 +594,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>58</v>
       </c>
       <c r="B7" s="2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>

</xml_diff>